<commit_message>
update figures 1 and 2
</commit_message>
<xml_diff>
--- a/data/flowchart.xlsx
+++ b/data/flowchart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daphneweemering/surfdrive/trial participation/meta-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daphneweemering/surfdrive/trial participation/trial-participation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FB3764-CF03-C642-B226-25E02A33A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F4D8EE-7F6E-8142-9F06-EB864046CC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BB2730CE-D5F6-824E-90DC-EA48B8B43E73}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{BB2730CE-D5F6-824E-90DC-EA48B8B43E73}"/>
   </bookViews>
   <sheets>
     <sheet name="OLD" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="41">
   <si>
     <t>Access to care</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>HCP-related factors</t>
+  </si>
+  <si>
+    <t>Medication administration</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F35778E-85AE-9340-AACA-2A6083515CBA}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -838,10 +841,7 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,21 +852,24 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
       </c>
       <c r="D27">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -874,10 +877,10 @@
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -885,10 +888,10 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -896,10 +899,10 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -907,9 +910,20 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
         <v>36</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>14</v>
       </c>
     </row>

</xml_diff>